<commit_message>
Modificari minore la workflows. Am scos majoritatea  message box urilor
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73669da328bd9310/Documents/UiPath/RoboticEnterpriseFramework_template_csharp/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{723AE724-DF2C-4EFA-8EBB-0881F67DFC56}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B664AD40-B62C-4A8E-A102-A47BFA80E628}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>The link for sandbox login</t>
+  </si>
+  <si>
+    <t>TransactionsFile</t>
+  </si>
+  <si>
+    <t>Data\Output\Transactions.csv</t>
+  </si>
+  <si>
+    <t>The path to LatestTransactions File</t>
   </si>
 </sst>
 </file>
@@ -1590,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1737,7 +1746,17 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>